<commit_message>
BOM & Model Tree Labels
</commit_message>
<xml_diff>
--- a/system_development/Mithril/v0.4/Mithril BOM.xlsx
+++ b/system_development/Mithril/v0.4/Mithril BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\In-situ-monitoring-of-powder-bed-fusion-additive-manufacturing\system_development\Mithril\v0.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9615772-8393-4E35-96E7-1E4BAC12E4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A312849-4B70-4FB7-ACE3-DAFA22F35104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,33 +92,15 @@
     <t>Aconity</t>
   </si>
   <si>
-    <t>M6x15</t>
-  </si>
-  <si>
-    <t>M6x20</t>
-  </si>
-  <si>
     <t>M6 ID 11.8mm OD Washer</t>
   </si>
   <si>
-    <t>M5x40</t>
-  </si>
-  <si>
     <t>M5 ID 9.8mm OD Washer</t>
   </si>
   <si>
-    <t>M4x14</t>
-  </si>
-  <si>
     <t>M4 ID 8.8mm OD Washer</t>
   </si>
   <si>
-    <t>M3x40</t>
-  </si>
-  <si>
-    <t>M3x10 Pan Head</t>
-  </si>
-  <si>
     <t>M3 Washer</t>
   </si>
   <si>
@@ -132,6 +114,24 @@
   </si>
   <si>
     <t>https://www.grainger.com/product/Rubber-Cord-Buna-N-848F88</t>
+  </si>
+  <si>
+    <t>M6x15 Bolt</t>
+  </si>
+  <si>
+    <t>M6x20 Bolt</t>
+  </si>
+  <si>
+    <t>M4x14 Bolt</t>
+  </si>
+  <si>
+    <t>M3x25 Bolt</t>
+  </si>
+  <si>
+    <t>M3x10 Pan Head Bolt</t>
+  </si>
+  <si>
+    <t>M5x40 Bolt</t>
   </si>
 </sst>
 </file>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +618,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
         <f>2</f>
@@ -627,7 +627,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1">
         <f>4</f>
@@ -636,7 +636,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <f>SUM(B13:B14)</f>
@@ -645,7 +645,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <f>B13</f>
@@ -654,7 +654,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1">
         <f>9+3</f>
@@ -663,7 +663,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <f ca="1">SUM(B17:B21)</f>
@@ -672,7 +672,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1">
         <f>3+4+4</f>
@@ -681,7 +681,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <f>B19</f>
@@ -690,7 +690,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1">
         <v>4</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <f>B22</f>
@@ -715,7 +715,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
@@ -723,13 +723,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>